<commit_message>
se termino el codigo de abrir y cerrar del reporte
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -41,13 +41,13 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>6/04/2021</x:t>
+    <x:t>1/03/2021</x:t>
   </x:si>
   <x:si>
     <x:t>FECHA FINAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>6/06/2021</x:t>
+    <x:t>9/06/2021</x:t>
   </x:si>
   <x:si>
     <x:t>MAQUINA</x:t>
@@ -141,7 +141,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </x:numFmts>
-  <x:fonts count="10" x14ac:knownFonts="1">
+  <x:fonts count="11" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -202,11 +202,17 @@
     </x:font>
     <x:font>
       <x:b/>
+      <x:sz val="12"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
       <x:sz val="10"/>
       <x:color theme="1"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
-      <x:scheme val="minor"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -589,87 +595,153 @@
     <x:xf numFmtId="0" fontId="7" fillId="0" borderId="25" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="19" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="18" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="15" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="11" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="15" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="14" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="24" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="19" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="18" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="15" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="11" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="15" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="14" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="42" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="63">
+  <x:cellXfs count="60">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="top"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center" wrapText="1"/>
     </x:xf>
@@ -694,7 +766,6 @@
     <x:xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center" wrapText="1"/>
     </x:xf>
@@ -708,36 +779,6 @@
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="top"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
     <x:xf numFmtId="42" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
@@ -753,51 +794,6 @@
     <x:xf numFmtId="42" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center" wrapText="1"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <x:xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
@@ -816,12 +812,15 @@
     <x:xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
     <x:xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="center" vertical="center"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -1165,10 +1164,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:N22"/>
+  <x:dimension ref="A1:N19"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <x:selection activeCell="L6" sqref="L6 L6:M7"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="O1" sqref="O1"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,432 +1188,539 @@
     <x:col min="14" max="14" width="1.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:14" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="1" spans="1:15" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A1" s="0">
         <x:f>A1:N19</x:f>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:14" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B2" s="15" t="s"/>
-      <x:c r="C2" s="17" t="s"/>
-      <x:c r="D2" s="17" t="s"/>
-      <x:c r="E2" s="17" t="s"/>
-      <x:c r="F2" s="17" t="s"/>
-      <x:c r="G2" s="17" t="s"/>
-      <x:c r="H2" s="17" t="s"/>
-      <x:c r="I2" s="17" t="s"/>
-      <x:c r="J2" s="17" t="s"/>
-      <x:c r="K2" s="17" t="s"/>
-      <x:c r="L2" s="17" t="s"/>
-      <x:c r="M2" s="17" t="s"/>
-      <x:c r="N2" s="18">
+    <x:row r="2" spans="1:15" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B2" s="22" t="s"/>
+      <x:c r="C2" s="20" t="s"/>
+      <x:c r="D2" s="20" t="s"/>
+      <x:c r="E2" s="20" t="s"/>
+      <x:c r="F2" s="20" t="s"/>
+      <x:c r="G2" s="20" t="s"/>
+      <x:c r="H2" s="20" t="s"/>
+      <x:c r="I2" s="20" t="s"/>
+      <x:c r="J2" s="20" t="s"/>
+      <x:c r="K2" s="20" t="s"/>
+      <x:c r="L2" s="20" t="s"/>
+      <x:c r="M2" s="20" t="s"/>
+      <x:c r="N2" s="19">
         <x:f>A45:N63</x:f>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:14" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B3" s="16" t="s"/>
-      <x:c r="C3" s="57" t="s"/>
-      <x:c r="D3" s="58" t="s"/>
-      <x:c r="E3" s="22" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F3" s="22" t="s"/>
-      <x:c r="G3" s="22" t="s"/>
-      <x:c r="H3" s="22" t="s"/>
-      <x:c r="I3" s="22" t="s"/>
-      <x:c r="J3" s="22" t="s"/>
-      <x:c r="K3" s="22" t="s"/>
-      <x:c r="L3" s="22" t="s"/>
-      <x:c r="M3" s="59" t="s"/>
-      <x:c r="N3" s="19" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:14" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B4" s="16" t="s"/>
-      <x:c r="C4" s="60" t="s"/>
-      <x:c r="D4" s="61" t="s"/>
-      <x:c r="E4" s="23" t="s">
+    <x:row r="3" spans="1:15" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B3" s="21" t="s"/>
+      <x:c r="C3" s="54" t="s"/>
+      <x:c r="D3" s="55" t="s"/>
+      <x:c r="E3" s="16" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F3" s="16" t="s"/>
+      <x:c r="G3" s="16" t="s"/>
+      <x:c r="H3" s="16" t="s"/>
+      <x:c r="I3" s="16" t="s"/>
+      <x:c r="J3" s="16" t="s"/>
+      <x:c r="K3" s="16" t="s"/>
+      <x:c r="L3" s="16" t="s"/>
+      <x:c r="M3" s="56" t="s"/>
+      <x:c r="N3" s="18" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B4" s="21" t="s"/>
+      <x:c r="C4" s="57" t="s"/>
+      <x:c r="D4" s="58" t="s"/>
+      <x:c r="E4" s="15" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F4" s="23" t="s"/>
-      <x:c r="G4" s="23" t="s"/>
-      <x:c r="H4" s="23" t="s"/>
-      <x:c r="I4" s="23" t="s"/>
-      <x:c r="J4" s="23" t="s"/>
-      <x:c r="K4" s="23" t="s"/>
-      <x:c r="L4" s="23" t="s"/>
-      <x:c r="M4" s="62" t="s"/>
-      <x:c r="N4" s="19" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:14" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B5" s="16" t="s"/>
-      <x:c r="C5" s="60" t="s"/>
-      <x:c r="D5" s="61" t="s"/>
-      <x:c r="E5" s="24" t="s">
+      <x:c r="F4" s="15" t="s"/>
+      <x:c r="G4" s="15" t="s"/>
+      <x:c r="H4" s="15" t="s"/>
+      <x:c r="I4" s="15" t="s"/>
+      <x:c r="J4" s="15" t="s"/>
+      <x:c r="K4" s="15" t="s"/>
+      <x:c r="L4" s="15" t="s"/>
+      <x:c r="M4" s="59" t="s"/>
+      <x:c r="N4" s="18" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:15" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B5" s="21" t="s"/>
+      <x:c r="C5" s="57" t="s"/>
+      <x:c r="D5" s="58" t="s"/>
+      <x:c r="E5" s="14" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="F5" s="24" t="s"/>
-      <x:c r="G5" s="24" t="s"/>
-      <x:c r="H5" s="24" t="s"/>
-      <x:c r="I5" s="24" t="s"/>
-      <x:c r="J5" s="24" t="s"/>
-      <x:c r="K5" s="24" t="s"/>
-      <x:c r="L5" s="24" t="s"/>
-      <x:c r="M5" s="62" t="s"/>
-      <x:c r="N5" s="19" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B6" s="16" t="s"/>
-      <x:c r="C6" s="40" t="s">
+      <x:c r="F5" s="14" t="s"/>
+      <x:c r="G5" s="14" t="s"/>
+      <x:c r="H5" s="14" t="s"/>
+      <x:c r="I5" s="14" t="s"/>
+      <x:c r="J5" s="14" t="s"/>
+      <x:c r="K5" s="14" t="s"/>
+      <x:c r="L5" s="14" t="s"/>
+      <x:c r="M5" s="59" t="s"/>
+      <x:c r="N5" s="18" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B6" s="21" t="s"/>
+      <x:c r="C6" s="13" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="D6" s="41" t="s"/>
-      <x:c r="E6" s="42" t="s"/>
-      <x:c r="F6" s="31" t="s">
+      <x:c r="D6" s="12" t="s"/>
+      <x:c r="E6" s="11" t="s"/>
+      <x:c r="F6" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="G6" s="31" t="s"/>
-      <x:c r="H6" s="31" t="s"/>
-      <x:c r="I6" s="31" t="s"/>
-      <x:c r="J6" s="32" t="s">
+      <x:c r="G6" s="7" t="s"/>
+      <x:c r="H6" s="7" t="s"/>
+      <x:c r="I6" s="7" t="s"/>
+      <x:c r="J6" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="K6" s="33" t="s"/>
-      <x:c r="L6" s="15" t="s">
+      <x:c r="K6" s="4" t="s"/>
+      <x:c r="L6" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="M6" s="18" t="s"/>
-      <x:c r="N6" s="19" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B7" s="16" t="s"/>
-      <x:c r="C7" s="36" t="s"/>
-      <x:c r="D7" s="37" t="s"/>
-      <x:c r="E7" s="38" t="s"/>
-      <x:c r="F7" s="30" t="s"/>
-      <x:c r="G7" s="30" t="s"/>
-      <x:c r="H7" s="30" t="s"/>
-      <x:c r="I7" s="30" t="s"/>
-      <x:c r="J7" s="34" t="s"/>
-      <x:c r="K7" s="35" t="s"/>
-      <x:c r="L7" s="39" t="s"/>
-      <x:c r="M7" s="20" t="s"/>
-      <x:c r="N7" s="19" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:14" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B8" s="16" t="s"/>
-      <x:c r="C8" s="2" t="s">
+      <x:c r="M6" s="4" t="s"/>
+      <x:c r="N6" s="18" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B7" s="21" t="s"/>
+      <x:c r="C7" s="10" t="s"/>
+      <x:c r="D7" s="9" t="s"/>
+      <x:c r="E7" s="8" t="s"/>
+      <x:c r="F7" s="6" t="s"/>
+      <x:c r="G7" s="6" t="s"/>
+      <x:c r="H7" s="6" t="s"/>
+      <x:c r="I7" s="6" t="s"/>
+      <x:c r="J7" s="3" t="s"/>
+      <x:c r="K7" s="2" t="s"/>
+      <x:c r="L7" s="3" t="s"/>
+      <x:c r="M7" s="2" t="s"/>
+      <x:c r="N7" s="18" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:15" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B8" s="21" t="s"/>
+      <x:c r="C8" s="24" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D8" s="1" t="s">
+      <x:c r="D8" s="23" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E8" s="2" t="s">
+      <x:c r="E8" s="24" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F8" s="6" t="s">
+      <x:c r="F8" s="28" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G8" s="2" t="s">
+      <x:c r="G8" s="24" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="H8" s="10" t="s">
+      <x:c r="H8" s="31" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="I8" s="2" t="s">
+      <x:c r="I8" s="24" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="J8" s="1" t="s">
+      <x:c r="J8" s="23" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="K8" s="2" t="s">
+      <x:c r="K8" s="24" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="L8" s="2" t="s">
+      <x:c r="L8" s="24" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="M8" s="11" t="s">
+      <x:c r="M8" s="32" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="N8" s="19" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B9" s="16" t="s"/>
-      <x:c r="C9" s="3" t="s">
+      <x:c r="N8" s="18" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B9" s="21" t="s"/>
+      <x:c r="C9" s="25" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D9" s="7" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E9" s="8" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F9" s="49" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G9" s="56" t="s"/>
-      <x:c r="H9" s="49" t="s"/>
-      <x:c r="I9" s="8" t="s"/>
-      <x:c r="J9" s="7" t="s"/>
-      <x:c r="K9" s="8" t="s"/>
-      <x:c r="L9" s="7" t="s"/>
-      <x:c r="M9" s="7">
+      <x:c r="D9" s="29" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E9" s="30" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F9" s="41" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G9" s="47" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H9" s="41" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I9" s="30" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J9" s="29" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K9" s="30" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L9" s="29" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M9" s="29">
         <x:f>+SUM(D9+E9+I9+J9+K9+L9)</x:f>
       </x:c>
-      <x:c r="N9" s="19" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B10" s="16" t="s"/>
-      <x:c r="C10" s="4" t="s">
+      <x:c r="N9" s="18" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B10" s="21" t="s"/>
+      <x:c r="C10" s="26" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D10" s="12" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E10" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F10" s="50" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G10" s="53" t="s"/>
-      <x:c r="H10" s="53" t="s"/>
-      <x:c r="I10" s="26" t="s"/>
-      <x:c r="J10" s="12" t="s"/>
-      <x:c r="K10" s="27" t="s"/>
-      <x:c r="L10" s="12" t="s"/>
-      <x:c r="M10" s="12">
+      <x:c r="D10" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E10" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F10" s="42" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G10" s="45" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H10" s="45" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I10" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J10" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K10" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L10" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M10" s="33">
         <x:f>+SUM(D10+E10+I10+J10+K10+L10)</x:f>
       </x:c>
-      <x:c r="N10" s="19" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B11" s="16" t="s"/>
-      <x:c r="C11" s="4" t="s">
+      <x:c r="N10" s="18" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B11" s="21" t="s"/>
+      <x:c r="C11" s="26" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D11" s="12" t="n">
+      <x:c r="D11" s="33" t="n">
+        <x:v>65000</x:v>
+      </x:c>
+      <x:c r="E11" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F11" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G11" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H11" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I11" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J11" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K11" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L11" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M11" s="33">
+        <x:f>+SUM(D11+E11+I11+J11+K11+L11)</x:f>
+      </x:c>
+      <x:c r="N11" s="18" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B12" s="21" t="s"/>
+      <x:c r="C12" s="26" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D12" s="33" t="n">
+        <x:v>500000</x:v>
+      </x:c>
+      <x:c r="E12" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F12" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G12" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H12" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I12" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J12" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K12" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L12" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M12" s="33">
+        <x:f>+SUM(D12+E12+I12+J12+K12+L12)</x:f>
+      </x:c>
+      <x:c r="N12" s="18" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B13" s="21" t="s"/>
+      <x:c r="C13" s="26" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D13" s="33" t="n">
         <x:v>45000</x:v>
       </x:c>
-      <x:c r="E11" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F11" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G11" s="54" t="s"/>
-      <x:c r="H11" s="54" t="s"/>
-      <x:c r="I11" s="26" t="s"/>
-      <x:c r="J11" s="12" t="s"/>
-      <x:c r="K11" s="27" t="s"/>
-      <x:c r="L11" s="12" t="s"/>
-      <x:c r="M11" s="12">
-        <x:f>+SUM(D11+E11+I11+J11+K11+L11)</x:f>
-      </x:c>
-      <x:c r="N11" s="19" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B12" s="16" t="s"/>
-      <x:c r="C12" s="4" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D12" s="12" t="n">
-        <x:v>500000</x:v>
-      </x:c>
-      <x:c r="E12" s="25" t="n">
-        <x:v>500000</x:v>
-      </x:c>
-      <x:c r="F12" s="51" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G12" s="54" t="s"/>
-      <x:c r="H12" s="54" t="s"/>
-      <x:c r="I12" s="26" t="s"/>
-      <x:c r="J12" s="12" t="s"/>
-      <x:c r="K12" s="27" t="s"/>
-      <x:c r="L12" s="12" t="s"/>
-      <x:c r="M12" s="12">
-        <x:f>+SUM(D12+E12+I12+J12+K12+L12)</x:f>
-      </x:c>
-      <x:c r="N12" s="19" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B13" s="16" t="s"/>
-      <x:c r="C13" s="4" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D13" s="12" t="n">
-        <x:v>45000</x:v>
-      </x:c>
-      <x:c r="E13" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F13" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G13" s="54" t="s"/>
-      <x:c r="H13" s="54" t="s"/>
-      <x:c r="I13" s="26" t="s"/>
-      <x:c r="J13" s="12" t="s"/>
-      <x:c r="K13" s="27" t="s"/>
-      <x:c r="L13" s="12" t="s"/>
-      <x:c r="M13" s="12">
+      <x:c r="E13" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F13" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G13" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H13" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I13" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J13" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K13" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L13" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M13" s="33">
         <x:f>+SUM(D13+E13+I13+J13+K13+L13)</x:f>
       </x:c>
-      <x:c r="N13" s="19" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B14" s="16" t="s"/>
-      <x:c r="C14" s="4" t="s">
+      <x:c r="N13" s="18" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B14" s="21" t="s"/>
+      <x:c r="C14" s="26" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D14" s="12" t="n">
+      <x:c r="D14" s="33" t="n">
         <x:v>50000</x:v>
       </x:c>
-      <x:c r="E14" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F14" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G14" s="54" t="s"/>
-      <x:c r="H14" s="54" t="s"/>
-      <x:c r="I14" s="26" t="s"/>
-      <x:c r="J14" s="12" t="s"/>
-      <x:c r="K14" s="27" t="s"/>
-      <x:c r="L14" s="12" t="s"/>
-      <x:c r="M14" s="12">
+      <x:c r="E14" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F14" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G14" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H14" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I14" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J14" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K14" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L14" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M14" s="33">
         <x:f>+SUM(D14+E14+I14+J14+K14+L14)</x:f>
       </x:c>
-      <x:c r="N14" s="19" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B15" s="16" t="s"/>
-      <x:c r="C15" s="4" t="s">
+      <x:c r="N14" s="18" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B15" s="21" t="s"/>
+      <x:c r="C15" s="26" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D15" s="12" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E15" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F15" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G15" s="54" t="s"/>
-      <x:c r="H15" s="54" t="s"/>
-      <x:c r="I15" s="26" t="s"/>
-      <x:c r="J15" s="12" t="s"/>
-      <x:c r="K15" s="27" t="s"/>
-      <x:c r="L15" s="12" t="s"/>
-      <x:c r="M15" s="12">
+      <x:c r="D15" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E15" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F15" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G15" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H15" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I15" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J15" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K15" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L15" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M15" s="33">
         <x:f>+SUM(D15+E15+I15+J15+K15+L15)</x:f>
       </x:c>
-      <x:c r="N15" s="19" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="B16" s="16" t="s"/>
-      <x:c r="C16" s="4" t="s">
+      <x:c r="N15" s="18" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="B16" s="21" t="s"/>
+      <x:c r="C16" s="26" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D16" s="12" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E16" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F16" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G16" s="54" t="s"/>
-      <x:c r="H16" s="54" t="s"/>
-      <x:c r="I16" s="26" t="s"/>
-      <x:c r="J16" s="12" t="s"/>
-      <x:c r="K16" s="27" t="s"/>
-      <x:c r="L16" s="12" t="s"/>
-      <x:c r="M16" s="12">
+      <x:c r="D16" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E16" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F16" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G16" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H16" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I16" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J16" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K16" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L16" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M16" s="33">
         <x:f>+SUM(D16+E16+I16+J16+K16+L16)</x:f>
       </x:c>
-      <x:c r="N16" s="19" t="s"/>
-    </x:row>
-    <x:row r="17" spans="1:14" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B17" s="16" t="s"/>
-      <x:c r="C17" s="4" t="s">
+      <x:c r="N16" s="18" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B17" s="21" t="s"/>
+      <x:c r="C17" s="26" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D17" s="12" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E17" s="25" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F17" s="51" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G17" s="54" t="s"/>
-      <x:c r="H17" s="54" t="s"/>
-      <x:c r="I17" s="26" t="s"/>
-      <x:c r="J17" s="12" t="s"/>
-      <x:c r="K17" s="27" t="s"/>
-      <x:c r="L17" s="28" t="s"/>
-      <x:c r="M17" s="28">
+      <x:c r="D17" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E17" s="36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F17" s="43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G17" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H17" s="46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I17" s="37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K17" s="38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L17" s="39" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="M17" s="39">
         <x:f>+SUM(D17+E17+I17+J17+K17+L17)</x:f>
       </x:c>
-      <x:c r="N17" s="19" t="s"/>
-    </x:row>
-    <x:row r="18" spans="1:14" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B18" s="16" t="s"/>
-      <x:c r="C18" s="5" t="s">
+      <x:c r="N17" s="18" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B18" s="21" t="s"/>
+      <x:c r="C18" s="27" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D18" s="29">
+      <x:c r="D18" s="40">
         <x:f>SUM(D9:D17)</x:f>
       </x:c>
-      <x:c r="E18" s="29">
+      <x:c r="E18" s="40">
         <x:f>SUM(E9:E17)</x:f>
       </x:c>
-      <x:c r="F18" s="52">
+      <x:c r="F18" s="44">
         <x:f>SUM(F9:F17)</x:f>
       </x:c>
-      <x:c r="G18" s="52">
+      <x:c r="G18" s="44">
         <x:f>SUM(G9:G17)</x:f>
       </x:c>
-      <x:c r="H18" s="52">
+      <x:c r="H18" s="44">
         <x:f>SUM(H9:H17)</x:f>
       </x:c>
-      <x:c r="I18" s="29">
+      <x:c r="I18" s="40">
         <x:f>SUM(I9:I17)</x:f>
       </x:c>
-      <x:c r="J18" s="29">
+      <x:c r="J18" s="40">
         <x:f>SUM(J9:J17)</x:f>
       </x:c>
-      <x:c r="K18" s="29">
+      <x:c r="K18" s="40">
         <x:f>SUM(K9:K17)</x:f>
       </x:c>
-      <x:c r="L18" s="29">
+      <x:c r="L18" s="40">
         <x:f>SUM(L9:L17)</x:f>
       </x:c>
-      <x:c r="M18" s="13">
+      <x:c r="M18" s="34">
         <x:f>+SUM(D18:L18)</x:f>
       </x:c>
-      <x:c r="N18" s="19" t="s"/>
-    </x:row>
-    <x:row r="19" spans="1:14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <x:c r="B19" s="14" t="s"/>
-      <x:c r="C19" s="21" t="s"/>
-      <x:c r="D19" s="21" t="s"/>
-      <x:c r="E19" s="21" t="s"/>
-      <x:c r="F19" s="21" t="s"/>
-      <x:c r="G19" s="21" t="s"/>
-      <x:c r="H19" s="21" t="s"/>
-      <x:c r="I19" s="21" t="s"/>
-      <x:c r="J19" s="21" t="s"/>
-      <x:c r="K19" s="21" t="s"/>
-      <x:c r="L19" s="21" t="s"/>
-      <x:c r="M19" s="21" t="s"/>
-      <x:c r="N19" s="20" t="s"/>
-    </x:row>
-    <x:row r="22" spans="1:14" x14ac:dyDescent="0.25"/>
+      <x:c r="N18" s="18" t="s"/>
+    </x:row>
+    <x:row r="19" spans="1:15" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="B19" s="35" t="s"/>
+      <x:c r="C19" s="1" t="s"/>
+      <x:c r="D19" s="1" t="s"/>
+      <x:c r="E19" s="1" t="s"/>
+      <x:c r="F19" s="1" t="s"/>
+      <x:c r="G19" s="1" t="s"/>
+      <x:c r="H19" s="1" t="s"/>
+      <x:c r="I19" s="1" t="s"/>
+      <x:c r="J19" s="1" t="s"/>
+      <x:c r="K19" s="1" t="s"/>
+      <x:c r="L19" s="1" t="s"/>
+      <x:c r="M19" s="1" t="s"/>
+      <x:c r="N19" s="17" t="s"/>
+    </x:row>
   </x:sheetData>
   <x:mergeCells count="11">
     <x:mergeCell ref="B2:B18"/>

</xml_diff>

<commit_message>
Se rastrea error en apertura y cierre de conexion
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>Q Y M S.A.S.</x:t>
   </x:si>
@@ -41,13 +41,10 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>1/03/2021</x:t>
+    <x:t>9/06/2021</x:t>
   </x:si>
   <x:si>
     <x:t>FECHA FINAL:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9/06/2021</x:t>
   </x:si>
   <x:si>
     <x:t>MAQUINA</x:t>
@@ -1279,7 +1276,7 @@
       </x:c>
       <x:c r="K6" s="4" t="s"/>
       <x:c r="L6" s="5" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M6" s="4" t="s"/>
       <x:c r="N6" s="18" t="s"/>
@@ -1302,47 +1299,47 @@
     <x:row r="8" spans="1:15" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B8" s="21" t="s"/>
       <x:c r="C8" s="24" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D8" s="23" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D8" s="23" t="s">
+      <x:c r="E8" s="24" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E8" s="24" t="s">
+      <x:c r="F8" s="28" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F8" s="28" t="s">
+      <x:c r="G8" s="24" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G8" s="24" t="s">
+      <x:c r="H8" s="31" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="H8" s="31" t="s">
+      <x:c r="I8" s="24" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="I8" s="24" t="s">
+      <x:c r="J8" s="23" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="J8" s="23" t="s">
+      <x:c r="K8" s="24" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="K8" s="24" t="s">
+      <x:c r="L8" s="24" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="L8" s="24" t="s">
+      <x:c r="M8" s="32" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="M8" s="32" t="s">
-        <x:v>17</x:v>
       </x:c>
       <x:c r="N8" s="18" t="s"/>
     </x:row>
     <x:row r="9" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B9" s="21" t="s"/>
       <x:c r="C9" s="25" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D9" s="29" t="n">
-        <x:v>0</x:v>
+        <x:v>45000</x:v>
       </x:c>
       <x:c r="E9" s="30" t="n">
         <x:v>0</x:v>
@@ -1376,10 +1373,10 @@
     <x:row r="10" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B10" s="21" t="s"/>
       <x:c r="C10" s="26" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E10" s="36" t="n">
         <x:v>0</x:v>
@@ -1413,10 +1410,10 @@
     <x:row r="11" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B11" s="21" t="s"/>
       <x:c r="C11" s="26" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D11" s="33" t="n">
-        <x:v>65000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E11" s="36" t="n">
         <x:v>0</x:v>
@@ -1450,10 +1447,10 @@
     <x:row r="12" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B12" s="21" t="s"/>
       <x:c r="C12" s="26" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D12" s="33" t="n">
-        <x:v>500000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E12" s="36" t="n">
         <x:v>0</x:v>
@@ -1487,10 +1484,10 @@
     <x:row r="13" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B13" s="21" t="s"/>
       <x:c r="C13" s="26" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D13" s="33" t="n">
-        <x:v>45000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E13" s="36" t="n">
         <x:v>0</x:v>
@@ -1524,10 +1521,10 @@
     <x:row r="14" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B14" s="21" t="s"/>
       <x:c r="C14" s="26" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D14" s="33" t="n">
-        <x:v>50000</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E14" s="36" t="n">
         <x:v>0</x:v>
@@ -1561,10 +1558,10 @@
     <x:row r="15" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B15" s="21" t="s"/>
       <x:c r="C15" s="26" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D15" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>50000</x:v>
       </x:c>
       <x:c r="E15" s="36" t="n">
         <x:v>0</x:v>
@@ -1598,10 +1595,10 @@
     <x:row r="16" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B16" s="21" t="s"/>
       <x:c r="C16" s="26" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D16" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E16" s="36" t="n">
         <x:v>0</x:v>
@@ -1635,10 +1632,10 @@
     <x:row r="17" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B17" s="21" t="s"/>
       <x:c r="C17" s="26" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D17" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E17" s="36" t="n">
         <x:v>0</x:v>
@@ -1672,7 +1669,7 @@
     <x:row r="18" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B18" s="21" t="s"/>
       <x:c r="C18" s="27" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D18" s="40">
         <x:f>SUM(D9:D17)</x:f>

</xml_diff>

<commit_message>
verificar lo de fredy
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -41,7 +41,7 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>1/03/2021</x:t>
+    <x:t>1/04/2021</x:t>
   </x:si>
   <x:si>
     <x:t>FECHA FINAL:</x:t>
@@ -1342,7 +1342,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="29" t="n">
-        <x:v>0</x:v>
+        <x:v>45000</x:v>
       </x:c>
       <x:c r="E9" s="30" t="n">
         <x:v>0</x:v>
@@ -1379,7 +1379,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="D10" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E10" s="36" t="n">
         <x:v>0</x:v>
@@ -1564,7 +1564,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="D15" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>50000</x:v>
       </x:c>
       <x:c r="E15" s="36" t="n">
         <x:v>0</x:v>
@@ -1601,7 +1601,7 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="D16" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E16" s="36" t="n">
         <x:v>0</x:v>
@@ -1638,7 +1638,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="D17" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E17" s="36" t="n">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
Se modifica abrir para la conexion maestra
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\datos\Documents\programa YA\QYMSASej - copia\QYMSAS\bin\Debug\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRG\source\repos\qymsas2\QYMSAS\bin\Debug\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FD40C8-7123-407F-9719-738C156363A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7590" firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <x:definedNames>
     <x:definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$N$19</x:definedName>
   </x:definedNames>
-  <x:calcPr calcId="162913"/>
+  <x:calcPr calcId="181029"/>
   <x:extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <x:si>
     <x:t>Q Y M S.A.S.</x:t>
   </x:si>
@@ -41,10 +42,13 @@
     <x:t>FECHA INICIAL:</x:t>
   </x:si>
   <x:si>
+    <x:t>9/01/2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FECHA FINAL:</x:t>
+  </x:si>
+  <x:si>
     <x:t>9/06/2021</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FECHA FINAL:</x:t>
   </x:si>
   <x:si>
     <x:t>MAQUINA</x:t>
@@ -134,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </x:numFmts>
@@ -1157,14 +1161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:N19"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="O1" sqref="O1"/>
+    <x:sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <x:selection activeCell="D11" sqref="D11"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,12 +1189,12 @@
     <x:col min="14" max="14" width="1.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:15" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="1" spans="1:14" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A1" s="0">
         <x:f>A1:N19</x:f>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:15" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="2" spans="1:14" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B2" s="22" t="s"/>
       <x:c r="C2" s="20" t="s"/>
       <x:c r="D2" s="20" t="s"/>
@@ -1207,7 +1211,7 @@
         <x:f>A45:N63</x:f>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:15" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="3" spans="1:14" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B3" s="21" t="s"/>
       <x:c r="C3" s="54" t="s"/>
       <x:c r="D3" s="55" t="s"/>
@@ -1224,7 +1228,7 @@
       <x:c r="M3" s="56" t="s"/>
       <x:c r="N3" s="18" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:14" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B4" s="21" t="s"/>
       <x:c r="C4" s="57" t="s"/>
       <x:c r="D4" s="58" t="s"/>
@@ -1241,7 +1245,7 @@
       <x:c r="M4" s="59" t="s"/>
       <x:c r="N4" s="18" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:15" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="5" spans="1:14" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B5" s="21" t="s"/>
       <x:c r="C5" s="57" t="s"/>
       <x:c r="D5" s="58" t="s"/>
@@ -1258,7 +1262,7 @@
       <x:c r="M5" s="59" t="s"/>
       <x:c r="N5" s="18" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B6" s="21" t="s"/>
       <x:c r="C6" s="13" t="s">
         <x:v>3</x:v>
@@ -1276,12 +1280,12 @@
       </x:c>
       <x:c r="K6" s="4" t="s"/>
       <x:c r="L6" s="5" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M6" s="4" t="s"/>
       <x:c r="N6" s="18" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="7" spans="1:14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B7" s="21" t="s"/>
       <x:c r="C7" s="10" t="s"/>
       <x:c r="D7" s="9" t="s"/>
@@ -1296,47 +1300,47 @@
       <x:c r="M7" s="2" t="s"/>
       <x:c r="N7" s="18" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:15" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="8" spans="1:14" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B8" s="21" t="s"/>
       <x:c r="C8" s="24" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="23" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E8" s="24" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="F8" s="28" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G8" s="24" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="H8" s="31" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="I8" s="24" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="J8" s="23" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="K8" s="24" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="L8" s="24" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M8" s="32" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="N8" s="18" t="s"/>
     </x:row>
-    <x:row r="9" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B9" s="21" t="s"/>
       <x:c r="C9" s="25" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="29" t="n">
         <x:v>45000</x:v>
@@ -1357,7 +1361,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="J9" s="29" t="n">
-        <x:v>0</x:v>
+        <x:v>70000</x:v>
       </x:c>
       <x:c r="K9" s="30" t="n">
         <x:v>0</x:v>
@@ -1370,10 +1374,10 @@
       </x:c>
       <x:c r="N9" s="18" t="s"/>
     </x:row>
-    <x:row r="10" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B10" s="21" t="s"/>
       <x:c r="C10" s="26" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D10" s="33" t="n">
         <x:v>500000</x:v>
@@ -1407,13 +1411,13 @@
       </x:c>
       <x:c r="N10" s="18" t="s"/>
     </x:row>
-    <x:row r="11" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="11" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B11" s="21" t="s"/>
       <x:c r="C11" s="26" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D11" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>65000</x:v>
       </x:c>
       <x:c r="E11" s="36" t="n">
         <x:v>0</x:v>
@@ -1428,13 +1432,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I11" s="37" t="n">
-        <x:v>0</x:v>
+        <x:v>1200000</x:v>
       </x:c>
       <x:c r="J11" s="33" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K11" s="38" t="n">
-        <x:v>0</x:v>
+        <x:v>25000</x:v>
       </x:c>
       <x:c r="L11" s="33" t="n">
         <x:v>0</x:v>
@@ -1444,28 +1448,28 @@
       </x:c>
       <x:c r="N11" s="18" t="s"/>
     </x:row>
-    <x:row r="12" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="12" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B12" s="21" t="s"/>
       <x:c r="C12" s="26" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D12" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="E12" s="36" t="n">
-        <x:v>0</x:v>
+        <x:v>500000</x:v>
       </x:c>
       <x:c r="F12" s="43" t="n">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G12" s="46" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="H12" s="46" t="n">
-        <x:v>0</x:v>
+        <x:v>800</x:v>
       </x:c>
       <x:c r="I12" s="37" t="n">
-        <x:v>0</x:v>
+        <x:v>2000000</x:v>
       </x:c>
       <x:c r="J12" s="33" t="n">
         <x:v>0</x:v>
@@ -1481,13 +1485,13 @@
       </x:c>
       <x:c r="N12" s="18" t="s"/>
     </x:row>
-    <x:row r="13" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B13" s="21" t="s"/>
       <x:c r="C13" s="26" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="D13" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>45000</x:v>
       </x:c>
       <x:c r="E13" s="36" t="n">
         <x:v>0</x:v>
@@ -1505,7 +1509,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="J13" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>50000</x:v>
       </x:c>
       <x:c r="K13" s="38" t="n">
         <x:v>0</x:v>
@@ -1518,13 +1522,13 @@
       </x:c>
       <x:c r="N13" s="18" t="s"/>
     </x:row>
-    <x:row r="14" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="14" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B14" s="21" t="s"/>
       <x:c r="C14" s="26" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D14" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>50000</x:v>
       </x:c>
       <x:c r="E14" s="36" t="n">
         <x:v>0</x:v>
@@ -1555,10 +1559,10 @@
       </x:c>
       <x:c r="N14" s="18" t="s"/>
     </x:row>
-    <x:row r="15" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B15" s="21" t="s"/>
       <x:c r="C15" s="26" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D15" s="33" t="n">
         <x:v>50000</x:v>
@@ -1573,7 +1577,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="H15" s="46" t="n">
-        <x:v>0</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="I15" s="37" t="n">
         <x:v>0</x:v>
@@ -1592,10 +1596,10 @@
       </x:c>
       <x:c r="N15" s="18" t="s"/>
     </x:row>
-    <x:row r="16" spans="1:15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="16" spans="1:14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B16" s="21" t="s"/>
       <x:c r="C16" s="26" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D16" s="33" t="n">
         <x:v>500000</x:v>
@@ -1629,10 +1633,10 @@
       </x:c>
       <x:c r="N16" s="18" t="s"/>
     </x:row>
-    <x:row r="17" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="17" spans="1:14" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B17" s="21" t="s"/>
       <x:c r="C17" s="26" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D17" s="33" t="n">
         <x:v>500000</x:v>
@@ -1666,10 +1670,10 @@
       </x:c>
       <x:c r="N17" s="18" t="s"/>
     </x:row>
-    <x:row r="18" spans="1:15" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="18" spans="1:14" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B18" s="21" t="s"/>
       <x:c r="C18" s="27" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D18" s="40">
         <x:f>SUM(D9:D17)</x:f>
@@ -1703,7 +1707,7 @@
       </x:c>
       <x:c r="N18" s="18" t="s"/>
     </x:row>
-    <x:row r="19" spans="1:15" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <x:row r="19" spans="1:14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="B19" s="35" t="s"/>
       <x:c r="C19" s="1" t="s"/>
       <x:c r="D19" s="1" t="s"/>

</xml_diff>

<commit_message>
se arreglo la linea de codigo del reporte en los viaticos
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -1474,7 +1474,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K12" s="38" t="n">
-        <x:v>0</x:v>
+        <x:v>47000</x:v>
       </x:c>
       <x:c r="L12" s="33" t="n">
         <x:v>0</x:v>
@@ -1514,7 +1514,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="L13" s="33" t="n">
-        <x:v>0</x:v>
+        <x:v>8000</x:v>
       </x:c>
       <x:c r="M13" s="33">
         <x:f>+SUM(D13+E13+I13+J13+K13+L13)</x:f>

</xml_diff>

<commit_message>
arreglo modificar y sha1 en la contraseña
</commit_message>
<xml_diff>
--- a/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
+++ b/QYMSAS/bin/Debug/temp/FMAQUINAS.xlsx
@@ -47,7 +47,7 @@
     <x:t>FECHA FINAL:</x:t>
   </x:si>
   <x:si>
-    <x:t>10/06/2021</x:t>
+    <x:t>14/06/2021</x:t>
   </x:si>
   <x:si>
     <x:t>MAQUINA</x:t>
@@ -1456,10 +1456,10 @@
         <x:v>500000</x:v>
       </x:c>
       <x:c r="E12" s="36" t="n">
-        <x:v>500000</x:v>
+        <x:v>1000000</x:v>
       </x:c>
       <x:c r="F12" s="43" t="n">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G12" s="46" t="n">
         <x:v>0</x:v>

</xml_diff>